<commit_message>
Merge branches 'acb1342' and 'leogon' of http://192.168.16.10:3388/mobilepark/hans
# Conflicts:
#	hans-core/src/main/java/com/mobilepark/doit5/admin/service/EquipmentService.java
#	hans-core/src/main/java/com/mobilepark/doit5/admin/service/EquipmentServiceImpl.java
</commit_message>
<xml_diff>
--- a/hans-sses/doc/SSES 테이블 정의서.xlsx
+++ b/hans-sses/doc/SSES 테이블 정의서.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29480" yWindow="740" windowWidth="35700" windowHeight="19060" tabRatio="500"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="35700" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sheet2" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="237">
   <si>
     <t>DATETIME</t>
   </si>
@@ -509,12 +509,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IDENTITY_CODE</t>
-  </si>
-  <si>
-    <t>식별코드</t>
-  </si>
-  <si>
     <t>BIRTHDAY</t>
   </si>
   <si>
@@ -737,12 +731,6 @@
     <t>로그정보</t>
   </si>
   <si>
-    <t>PART_CODE</t>
-  </si>
-  <si>
-    <t>구분코드</t>
-  </si>
-  <si>
     <t>VALUE</t>
   </si>
   <si>
@@ -848,10 +836,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ELECT_POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -869,6 +853,46 @@
   </si>
   <si>
     <t>COMPANY_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EQUIP_SEQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USER_SEQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자SEQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근태관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBL_ATTENDANCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST_DATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접속구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접속날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -933,7 +957,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,6 +967,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,12 +1160,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1224,11 +1256,94 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="56" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="기본" xfId="0" builtinId="0"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="3" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1503,15 +1618,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H180"/>
+  <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="J89" sqref="J89"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A125" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I147" sqref="I147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -1519,7 +1634,7 @@
     <col min="6" max="6" width="7.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="7.5703125" style="7"/>
+    <col min="9" max="16384" width="7.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1562,11 +1677,11 @@
       <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -1755,7 +1870,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>52</v>
@@ -1810,11 +1925,11 @@
       <c r="A15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -1939,7 +2054,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>52</v>
@@ -1994,11 +2109,11 @@
       <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -2129,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>52</v>
@@ -2184,11 +2299,11 @@
       <c r="A33" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2376,7 +2491,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>52</v>
@@ -2431,11 +2546,11 @@
       <c r="A45" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -2642,7 +2757,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>52</v>
@@ -2697,11 +2812,11 @@
       <c r="A58" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -2738,7 +2853,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>101</v>
@@ -2890,7 +3005,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>52</v>
@@ -2945,11 +3060,11 @@
       <c r="A70" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C70" s="29"/>
-      <c r="D70" s="29"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
@@ -3019,7 +3134,7 @@
         <v>29</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>92</v>
@@ -3158,7 +3273,7 @@
         <v>9</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>52</v>
@@ -3196,7 +3311,7 @@
         <v>14</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>16</v>
@@ -3213,11 +3328,11 @@
       <c r="A83" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B83" s="29" t="s">
+      <c r="B83" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
@@ -3254,7 +3369,7 @@
         <v>1</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>122</v>
@@ -3301,7 +3416,7 @@
         <v>95</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>29</v>
@@ -3320,7 +3435,7 @@
         <v>4</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>125</v>
@@ -3366,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C90" s="18" t="s">
         <v>52</v>
@@ -3421,11 +3536,11 @@
       <c r="A93" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B93" s="29" t="s">
+      <c r="B93" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="29"/>
-      <c r="D93" s="29"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
@@ -3462,16 +3577,16 @@
         <v>1</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>128</v>
+        <v>229</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>129</v>
+        <v>230</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E95" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F95" s="15" t="s">
         <v>31</v>
@@ -3486,7 +3601,7 @@
         <v>2</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>122</v>
@@ -3510,16 +3625,16 @@
         <v>4</v>
       </c>
       <c r="B97" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E97" s="15" t="s">
-        <v>132</v>
       </c>
       <c r="F97" s="16"/>
       <c r="G97" s="16"/>
@@ -3530,10 +3645,10 @@
         <v>5</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>29</v>
@@ -3555,13 +3670,13 @@
         <v>41</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E99" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F99" s="15" t="s">
         <v>31</v>
@@ -3574,10 +3689,10 @@
         <v>7</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>29</v>
@@ -3594,16 +3709,16 @@
         <v>8</v>
       </c>
       <c r="B101" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C101" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="15" t="s">
         <v>138</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D101" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E101" s="15" t="s">
-        <v>140</v>
       </c>
       <c r="F101" s="16"/>
       <c r="G101" s="16"/>
@@ -3614,10 +3729,10 @@
         <v>9</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>29</v>
@@ -3634,10 +3749,10 @@
         <v>10</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D103" s="15" t="s">
         <v>29</v>
@@ -3678,7 +3793,7 @@
         <v>12</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C105" s="18" t="s">
         <v>52</v>
@@ -3698,7 +3813,7 @@
         <v>11</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>13</v>
@@ -3716,7 +3831,7 @@
         <v>14</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>16</v>
@@ -3733,11 +3848,11 @@
       <c r="A108" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B108" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C108" s="29"/>
-      <c r="D108" s="29"/>
+      <c r="B108" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C108" s="30"/>
+      <c r="D108" s="30"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
       <c r="G108" s="11"/>
@@ -3774,10 +3889,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>29</v>
@@ -3798,10 +3913,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>29</v>
@@ -3820,16 +3935,16 @@
         <v>3</v>
       </c>
       <c r="B112" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E112" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="D112" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E112" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="F112" s="15" t="s">
         <v>31</v>
@@ -3842,16 +3957,16 @@
         <v>4</v>
       </c>
       <c r="B113" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E113" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D113" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E113" s="15" t="s">
-        <v>157</v>
       </c>
       <c r="F113" s="15" t="s">
         <v>31</v>
@@ -3888,7 +4003,7 @@
         <v>6</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C115" s="18" t="s">
         <v>52</v>
@@ -3908,7 +4023,7 @@
         <v>11</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>13</v>
@@ -3926,7 +4041,7 @@
         <v>14</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>16</v>
@@ -3943,11 +4058,11 @@
       <c r="A118" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B118" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C118" s="29"/>
-      <c r="D118" s="29"/>
+      <c r="B118" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C118" s="30"/>
+      <c r="D118" s="30"/>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
       <c r="G118" s="11"/>
@@ -3984,16 +4099,16 @@
         <v>1</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E120" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F120" s="15" t="s">
         <v>31</v>
@@ -4011,13 +4126,13 @@
         <v>41</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E121" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F121" s="15" t="s">
         <v>31</v>
@@ -4030,16 +4145,16 @@
         <v>3</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E122" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F122" s="16"/>
       <c r="G122" s="16"/>
@@ -4050,16 +4165,16 @@
         <v>4</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E123" s="15" t="s">
-        <v>226</v>
+        <v>64</v>
       </c>
       <c r="F123" s="16"/>
       <c r="G123" s="16"/>
@@ -4070,16 +4185,16 @@
         <v>5</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E124" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F124" s="16"/>
       <c r="G124" s="16"/>
@@ -4090,16 +4205,16 @@
         <v>6</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E125" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F125" s="15" t="s">
         <v>31</v>
@@ -4134,7 +4249,7 @@
         <v>8</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C127" s="18" t="s">
         <v>52</v>
@@ -4154,7 +4269,7 @@
         <v>11</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>13</v>
@@ -4172,7 +4287,7 @@
         <v>14</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C129" s="10" t="s">
         <v>16</v>
@@ -4189,11 +4304,11 @@
       <c r="A130" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B130" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="C130" s="29"/>
-      <c r="D130" s="29"/>
+      <c r="B130" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C130" s="30"/>
+      <c r="D130" s="30"/>
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
       <c r="G130" s="11"/>
@@ -4230,16 +4345,16 @@
         <v>1</v>
       </c>
       <c r="B132" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E132" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F132" s="15" t="s">
         <v>31</v>
@@ -4254,16 +4369,16 @@
         <v>2</v>
       </c>
       <c r="B133" s="15" t="s">
-        <v>128</v>
+        <v>229</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>129</v>
+        <v>230</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E133" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F133" s="15" t="s">
         <v>31</v>
@@ -4278,16 +4393,16 @@
         <v>3</v>
       </c>
       <c r="B134" s="15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E134" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F134" s="15" t="s">
         <v>31</v>
@@ -4302,16 +4417,16 @@
         <v>4</v>
       </c>
       <c r="B135" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E135" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F135" s="15" t="s">
         <v>31</v>
@@ -4346,7 +4461,7 @@
         <v>6</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C137" s="18" t="s">
         <v>52</v>
@@ -4366,7 +4481,7 @@
         <v>11</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>13</v>
@@ -4384,7 +4499,7 @@
         <v>14</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C139" s="10" t="s">
         <v>16</v>
@@ -4401,11 +4516,11 @@
       <c r="A140" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B140" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="C140" s="29"/>
-      <c r="D140" s="29"/>
+      <c r="B140" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="C140" s="30"/>
+      <c r="D140" s="30"/>
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
       <c r="G140" s="11"/>
@@ -4442,16 +4557,16 @@
         <v>1</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D142" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E142" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F142" s="15" t="s">
         <v>31</v>
@@ -4469,13 +4584,13 @@
         <v>3</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D143" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E143" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F143" s="15" t="s">
         <v>31</v>
@@ -4491,13 +4606,13 @@
         <v>2</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D144" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E144" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F144" s="15" t="s">
         <v>31</v>
@@ -4510,16 +4625,16 @@
         <v>4</v>
       </c>
       <c r="B145" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D145" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E145" s="15" t="s">
         <v>189</v>
-      </c>
-      <c r="C145" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D145" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E145" s="15" t="s">
-        <v>191</v>
       </c>
       <c r="F145" s="15" t="s">
         <v>31</v>
@@ -4532,16 +4647,16 @@
         <v>5</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D146" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E146" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F146" s="15"/>
       <c r="G146" s="16">
@@ -4557,7 +4672,7 @@
         <v>27</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D147" s="15" t="s">
         <v>29</v>
@@ -4576,20 +4691,20 @@
         <v>7</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D148" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E148" s="15" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F148" s="15"/>
       <c r="G148" s="16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H148" s="20"/>
     </row>
@@ -4607,7 +4722,7 @@
         <v>29</v>
       </c>
       <c r="E149" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F149" s="15" t="s">
         <v>31</v>
@@ -4620,7 +4735,7 @@
         <v>9</v>
       </c>
       <c r="B150" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C150" s="18" t="s">
         <v>52</v>
@@ -4629,7 +4744,7 @@
         <v>29</v>
       </c>
       <c r="E150" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F150" s="18"/>
       <c r="G150" s="19"/>
@@ -4640,7 +4755,7 @@
         <v>11</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>13</v>
@@ -4658,7 +4773,7 @@
         <v>14</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C152" s="10" t="s">
         <v>16</v>
@@ -4675,11 +4790,11 @@
       <c r="A153" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B153" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="C153" s="29"/>
-      <c r="D153" s="29"/>
+      <c r="B153" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C153" s="30"/>
+      <c r="D153" s="30"/>
       <c r="E153" s="11"/>
       <c r="F153" s="11"/>
       <c r="G153" s="11"/>
@@ -4716,16 +4831,16 @@
         <v>1</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D155" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E155" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F155" s="15" t="s">
         <v>31</v>
@@ -4735,15 +4850,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="14">
         <v>2</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>129</v>
+        <v>228</v>
       </c>
       <c r="D156" s="15" t="s">
         <v>29</v>
@@ -4755,47 +4870,47 @@
         <v>31</v>
       </c>
       <c r="G156" s="16"/>
-      <c r="H156" s="20" t="s">
+      <c r="H156" s="20"/>
+    </row>
+    <row r="157" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>2</v>
+      </c>
+      <c r="B157" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C157" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D157" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E157" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F157" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G157" s="16"/>
+      <c r="H157" s="20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A157" s="14">
-        <v>3</v>
-      </c>
-      <c r="B157" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C157" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="D157" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E157" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F157" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G157" s="16"/>
-      <c r="H157" s="17"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="D158" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E158" s="15" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="F158" s="15" t="s">
         <v>31</v>
@@ -4804,468 +4919,705 @@
       <c r="H158" s="17"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A159" s="24">
-        <v>5</v>
-      </c>
-      <c r="B159" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="C159" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="D159" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="E159" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="F159" s="25"/>
-      <c r="G159" s="26"/>
-      <c r="H159" s="27"/>
+      <c r="A159" s="14">
+        <v>4</v>
+      </c>
+      <c r="B159" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C159" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D159" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E159" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F159" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G159" s="16"/>
+      <c r="H159" s="17"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="24">
-        <v>6</v>
-      </c>
-      <c r="B160" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C160" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D160" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E160" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="F160" s="15" t="s">
-        <v>31</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B160" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C160" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D160" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E160" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="F160" s="25"/>
       <c r="G160" s="26"/>
       <c r="H160" s="27"/>
     </row>
-    <row r="161" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="21">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="24">
+        <v>6</v>
+      </c>
+      <c r="B161" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C161" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D161" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E161" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F161" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G161" s="26"/>
+      <c r="H161" s="27"/>
+    </row>
+    <row r="162" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="21">
         <v>7</v>
       </c>
-      <c r="B161" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="C161" s="18" t="s">
+      <c r="B162" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C162" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D161" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E161" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="F161" s="18"/>
-      <c r="G161" s="19"/>
-      <c r="H161" s="22"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+      <c r="D162" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E162" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F162" s="18"/>
+      <c r="G162" s="19"/>
+      <c r="H162" s="22"/>
+    </row>
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B163" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C163" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" s="34">
+        <v>42800</v>
+      </c>
+      <c r="E163" s="35"/>
+      <c r="F163" s="35"/>
+      <c r="G163" s="35"/>
+      <c r="H163" s="36"/>
+    </row>
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B164" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C164" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D164" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E164" s="40"/>
+      <c r="F164" s="40"/>
+      <c r="G164" s="40"/>
+      <c r="H164" s="41"/>
+    </row>
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B165" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="C165" s="42"/>
+      <c r="D165" s="42"/>
+      <c r="E165" s="40"/>
+      <c r="F165" s="40"/>
+      <c r="G165" s="40"/>
+      <c r="H165" s="41"/>
+    </row>
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B166" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C166" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D166" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E166" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F166" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="G166" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H166" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="44">
+        <v>1</v>
+      </c>
+      <c r="B167" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C167" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D167" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E167" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="F167" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G167" s="46"/>
+      <c r="H167" s="47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="44">
+        <v>2</v>
+      </c>
+      <c r="B168" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="C168" s="45" t="s">
+        <v>230</v>
+      </c>
+      <c r="D168" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E168" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F168" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G168" s="46"/>
+      <c r="H168" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="44">
+        <v>3</v>
+      </c>
+      <c r="B169" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="C162" s="3" t="s">
+      <c r="C169" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="D169" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E169" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F169" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G169" s="46"/>
+      <c r="H169" s="48"/>
+    </row>
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="44">
+        <v>4</v>
+      </c>
+      <c r="B170" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C170" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D170" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E170" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="F170" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G170" s="46"/>
+      <c r="H170" s="48"/>
+    </row>
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="49">
+        <v>5</v>
+      </c>
+      <c r="B171" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C171" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D171" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E171" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="F171" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G171" s="50"/>
+      <c r="H171" s="51"/>
+    </row>
+    <row r="172" spans="1:8" ht="19" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="52">
+        <v>6</v>
+      </c>
+      <c r="B172" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="C172" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D172" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E172" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="F172" s="53"/>
+      <c r="G172" s="54"/>
+      <c r="H172" s="55"/>
+    </row>
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B173" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C173" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D162" s="4">
-        <v>42800</v>
-      </c>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
-      <c r="H162" s="6"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A163" s="8" t="s">
+      <c r="D173" s="56">
+        <v>42816</v>
+      </c>
+      <c r="E173" s="35"/>
+      <c r="F173" s="35"/>
+      <c r="G173" s="35"/>
+      <c r="H173" s="36"/>
+    </row>
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B163" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="C163" s="10" t="s">
+      <c r="B174" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="C174" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D163" s="23" t="s">
+      <c r="D174" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E163" s="11"/>
-      <c r="F163" s="11"/>
-      <c r="G163" s="11"/>
-      <c r="H163" s="12"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A164" s="8" t="s">
+      <c r="E174" s="40"/>
+      <c r="F174" s="40"/>
+      <c r="G174" s="40"/>
+      <c r="H174" s="41"/>
+    </row>
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B164" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="C164" s="29"/>
-      <c r="D164" s="29"/>
-      <c r="E164" s="11"/>
-      <c r="F164" s="11"/>
-      <c r="G164" s="11"/>
-      <c r="H164" s="12"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A165" s="8" t="s">
+      <c r="B175" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C175" s="42"/>
+      <c r="D175" s="42"/>
+      <c r="E175" s="40"/>
+      <c r="F175" s="40"/>
+      <c r="G175" s="40"/>
+      <c r="H175" s="41"/>
+    </row>
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B165" s="10" t="s">
+      <c r="B176" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C165" s="10" t="s">
+      <c r="C176" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D165" s="10" t="s">
+      <c r="D176" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E165" s="10" t="s">
+      <c r="E176" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F165" s="10" t="s">
+      <c r="F176" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="G165" s="10" t="s">
+      <c r="G176" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="H165" s="13" t="s">
+      <c r="H176" s="43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A166" s="14">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="44">
         <v>1</v>
       </c>
-      <c r="B166" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C166" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D166" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E166" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="F166" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G166" s="16"/>
-      <c r="H166" s="20" t="s">
+      <c r="B177" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C177" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D177" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E177" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="F177" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G177" s="46"/>
+      <c r="H177" s="47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A167" s="14">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="44">
         <v>2</v>
       </c>
-      <c r="B167" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C167" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D167" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E167" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F167" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G167" s="16"/>
-      <c r="H167" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A168" s="14">
+      <c r="B178" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C178" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="D178" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E178" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="F178" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G178" s="46"/>
+      <c r="H178" s="47"/>
+    </row>
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="44">
         <v>3</v>
       </c>
-      <c r="B168" s="15" t="s">
+      <c r="B179" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C168" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D168" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E168" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F168" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G168" s="16"/>
-      <c r="H168" s="17"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" s="14">
+      <c r="C179" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D179" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E179" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="F179" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G179" s="46"/>
+      <c r="H179" s="48"/>
+    </row>
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="49">
         <v>4</v>
       </c>
-      <c r="B169" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C169" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D169" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E169" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="F169" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G169" s="16"/>
-      <c r="H169" s="17"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" s="24">
+      <c r="B180" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C180" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D180" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E180" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="F180" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G180" s="50"/>
+      <c r="H180" s="51"/>
+    </row>
+    <row r="181" spans="1:8" ht="19" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="52">
         <v>5</v>
       </c>
-      <c r="B170" s="15" t="s">
+      <c r="B181" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="C181" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D181" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E181" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="F181" s="53"/>
+      <c r="G181" s="54"/>
+      <c r="H181" s="55"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D182" s="28">
+        <v>42828</v>
+      </c>
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+      <c r="G182" s="5"/>
+      <c r="H182" s="6"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B183" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="C183" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D183" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E183" s="11"/>
+      <c r="F183" s="11"/>
+      <c r="G183" s="11"/>
+      <c r="H183" s="12"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B184" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C184" s="30"/>
+      <c r="D184" s="30"/>
+      <c r="E184" s="11"/>
+      <c r="F184" s="11"/>
+      <c r="G184" s="11"/>
+      <c r="H184" s="12"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C185" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E185" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F185" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G185" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H185" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>1</v>
+      </c>
+      <c r="B186" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C186" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D186" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E186" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F186" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G186" s="16"/>
+      <c r="H186" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>2</v>
+      </c>
+      <c r="B187" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C187" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D187" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E187" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F187" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G187" s="16"/>
+      <c r="H187" s="20"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>2</v>
+      </c>
+      <c r="B188" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C188" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D188" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E188" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="F188" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G188" s="16"/>
+      <c r="H188" s="20"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>3</v>
+      </c>
+      <c r="B189" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C189" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D189" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E189" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F189" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G189" s="16"/>
+      <c r="H189" s="17"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="24">
+        <v>6</v>
+      </c>
+      <c r="B190" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C170" s="15" t="s">
+      <c r="C190" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D170" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E170" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="F170" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G170" s="26"/>
-      <c r="H170" s="27"/>
-    </row>
-    <row r="171" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="21">
-        <v>6</v>
-      </c>
-      <c r="B171" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="C171" s="18" t="s">
+      <c r="D190" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E190" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F190" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G190" s="26"/>
+      <c r="H190" s="27"/>
+    </row>
+    <row r="191" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="21">
+        <v>7</v>
+      </c>
+      <c r="B191" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C191" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D171" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E171" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="F171" s="18"/>
-      <c r="G171" s="19"/>
-      <c r="H171" s="22"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D172" s="28">
-        <v>42816</v>
-      </c>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
-      <c r="H172" s="6"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A173" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B173" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="C173" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D173" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E173" s="11"/>
-      <c r="F173" s="11"/>
-      <c r="G173" s="11"/>
-      <c r="H173" s="12"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B174" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="C174" s="29"/>
-      <c r="D174" s="29"/>
-      <c r="E174" s="11"/>
-      <c r="F174" s="11"/>
-      <c r="G174" s="11"/>
-      <c r="H174" s="12"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B175" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C175" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D175" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E175" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F175" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G175" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H175" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A176" s="14">
-        <v>1</v>
-      </c>
-      <c r="B176" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C176" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D176" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E176" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="F176" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G176" s="16"/>
-      <c r="H176" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A177" s="14">
-        <v>2</v>
-      </c>
-      <c r="B177" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="C177" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D177" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E177" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="F177" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G177" s="16"/>
-      <c r="H177" s="20"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A178" s="14">
-        <v>3</v>
-      </c>
-      <c r="B178" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D178" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E178" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="F178" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G178" s="16"/>
-      <c r="H178" s="17"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A179" s="24">
-        <v>4</v>
-      </c>
-      <c r="B179" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C179" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D179" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E179" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="F179" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G179" s="26"/>
-      <c r="H179" s="27"/>
-    </row>
-    <row r="180" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="21">
-        <v>5</v>
-      </c>
-      <c r="B180" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="C180" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D180" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E180" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="F180" s="18"/>
-      <c r="G180" s="19"/>
-      <c r="H180" s="22"/>
+      <c r="D191" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E191" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F191" s="18"/>
+      <c r="G191" s="19"/>
+      <c r="H191" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B45:D45"/>
     <mergeCell ref="B153:D153"/>
-    <mergeCell ref="B164:D164"/>
-    <mergeCell ref="B174:D174"/>
+    <mergeCell ref="B165:D165"/>
+    <mergeCell ref="B175:D175"/>
     <mergeCell ref="B140:D140"/>
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B83:D83"/>
@@ -5273,12 +5625,6 @@
     <mergeCell ref="B108:D108"/>
     <mergeCell ref="B118:D118"/>
     <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>